<commit_message>
[main] Set prescaler and counter period of TIM21(1ms) and TIM22(1us) below.
- TIM21, 1ms, prescaler[3199], counter period[9]
- TIM22, 1us, prescaler[31], counter period[65535]
- Verify by __MEASURE_TIM22
</commit_message>
<xml_diff>
--- a/Document/Environment.xlsx
+++ b/Document/Environment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\GSL\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9D7F69-4C14-4FB2-8476-93EA0514B434}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723072B3-6274-485C-921C-12C6A2875443}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1" xr2:uid="{2B8BF1E6-E496-4F89-BDC8-54DCCB78AA27}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t>GTK</t>
   </si>
@@ -105,10 +105,82 @@
     <t>PWM Setting</t>
   </si>
   <si>
-    <t>Frequency(MHz)</t>
-  </si>
-  <si>
     <t>Prescaler</t>
+  </si>
+  <si>
+    <t>Counter Period</t>
+  </si>
+  <si>
+    <t>PWM Output</t>
+  </si>
+  <si>
+    <t>https://qiita.com/ShunHattori/items/68f099f1d77702d2535d</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>https://community.st.com/t5/stm32-mcus/how-to-use-stlink-v3-mco-output-on-nucleo-boards-as-a-precise/ta-p/723361</t>
+  </si>
+  <si>
+    <t>ISR?(Cortex M3)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/16656489/safely-detect-if-function-is-called-from-an-isr</t>
+  </si>
+  <si>
+    <t>https://www.renesas.com/en/document/mah/idt-arm-cortex-m0-user-guide</t>
+  </si>
+  <si>
+    <t>CubeIDE(Split peripherals)</t>
+  </si>
+  <si>
+    <t>https://community.st.com/t5/stm32cubemx-mcus/is-it-possible-to-automatically-separate-the-code-generated-by/td-p/71174</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>after</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>RAM(KB)</t>
+  </si>
+  <si>
+    <t>ROM(KB)</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>gts_feature.h</t>
+  </si>
+  <si>
+    <t>GTK_SC_PERIPHERALS [SHA-1: 3deb3aa8da26ad4805db492b78408d75ca17b15b]</t>
+  </si>
+  <si>
+    <t>GTK_SC_BASE [SHA-1: 74b4d3d425f102277975e83fb277a20295cfb6da]</t>
+  </si>
+  <si>
+    <t>GTK_SC_PERIPHERALS Implemented [SHA-1: 3deb3aa8da26ad4805db492b78408d75ca17b15b]</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>https://qiita.com/numeru55/items/fd61922eeec6be62a22a</t>
+  </si>
+  <si>
+    <t>Measure execution time</t>
+  </si>
+  <si>
+    <t>https://www.iar.com/knowledge/learn/debugging/techniques-for-measuring-the-elapsed-timeew-page/</t>
+  </si>
+  <si>
+    <t>Frequency(Hz)</t>
   </si>
   <si>
     <r>
@@ -135,113 +207,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(KHz)</t>
+      <t>(Hz)</t>
     </r>
   </si>
   <si>
-    <t>Counter Period</t>
-  </si>
-  <si>
-    <t>PWM Output</t>
-  </si>
-  <si>
-    <t>https://qiita.com/ShunHattori/items/68f099f1d77702d2535d</t>
-  </si>
-  <si>
-    <t>Clock</t>
-  </si>
-  <si>
-    <t>https://community.st.com/t5/stm32-mcus/how-to-use-stlink-v3-mco-output-on-nucleo-boards-as-a-precise/ta-p/723361</t>
-  </si>
-  <si>
-    <t>ISR?(Cortex M3)</t>
-  </si>
-  <si>
-    <t>https://stackoverflow.com/questions/16656489/safely-detect-if-function-is-called-from-an-isr</t>
-  </si>
-  <si>
-    <t>https://www.renesas.com/en/document/mah/idt-arm-cortex-m0-user-guide</t>
-  </si>
-  <si>
-    <t>CubeIDE(Split peripherals)</t>
-  </si>
-  <si>
-    <t>https://community.st.com/t5/stm32cubemx-mcus/is-it-possible-to-automatically-separate-the-code-generated-by/td-p/71174</t>
-  </si>
-  <si>
-    <t>before</t>
-  </si>
-  <si>
-    <t>after</t>
-  </si>
-  <si>
-    <t>diff</t>
-  </si>
-  <si>
-    <t>RAM(KB)</t>
-  </si>
-  <si>
-    <t>ROM(KB)</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>gts_feature.h</t>
-  </si>
-  <si>
-    <t>GTK_SC_PERIPHERALS [SHA-1: 3deb3aa8da26ad4805db492b78408d75ca17b15b]</t>
-  </si>
-  <si>
-    <t>GTK_SC_BASE [SHA-1: 74b4d3d425f102277975e83fb277a20295cfb6da]</t>
-  </si>
-  <si>
-    <t>GTK_SC_PERIPHERALS Implemented [SHA-1: 3deb3aa8da26ad4805db492b78408d75ca17b15b]</t>
-  </si>
-  <si>
-    <t>UART</t>
-  </si>
-  <si>
-    <t>https://qiita.com/numeru55/items/fd61922eeec6be62a22a</t>
-  </si>
-  <si>
-    <t>Measure execution time</t>
-  </si>
-  <si>
-    <t>https://www.iar.com/knowledge/learn/debugging/techniques-for-measuring-the-elapsed-timeew-page/</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[0]</t>
-  </si>
-  <si>
-    <t>unsigned long</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[1]</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[2]</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[3]</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[4]</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[5]</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[6]</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[7]</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[8]</t>
-  </si>
-  <si>
-    <t>u32Tick22_1u[9]</t>
+    <t>1ms</t>
+  </si>
+  <si>
+    <t>1us</t>
   </si>
 </sst>
 </file>
@@ -878,7 +851,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -952,10 +925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777F88CA-E307-47AA-93AB-8788864B7E3B}">
-  <dimension ref="B2:G32"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,205 +939,138 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3">
+        <f>32*1000*1000</f>
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3">
+        <f>C10/(C13+1)/(C11+1)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3">
-        <f>$C$10*1000*1000/($C$13+1)/($C$11+1)</f>
-        <v>14.796401515151516</v>
-      </c>
-      <c r="D12">
-        <f>1/C12</f>
-        <v>6.7583999999999991E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" s="3">
+        <v>31999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="3">
+        <f>32*1000*1000</f>
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="3">
+        <f>C16/(C19+1)/(C17+1)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="3">
+        <f>32*1000*1000</f>
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="3">
+        <f>C22/(C25+1)/(C23+1)</f>
+        <v>15.2587890625</v>
+      </c>
+      <c r="D24">
+        <f>1/C24</f>
+        <v>6.5535999999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3">
         <v>65535</v>
       </c>
-      <c r="D13">
-        <f>D12/C13</f>
-        <v>1.0312657358663308E-6</v>
-      </c>
-      <c r="E13">
-        <f>D13*1000</f>
-        <v>1.0312657358663307E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <f>F24-F23</f>
-        <v>972</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24">
-        <v>972</v>
-      </c>
-      <c r="G24">
-        <f t="shared" ref="G24:G32" si="0">F25-F24</f>
-        <v>970</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25">
-        <v>1942</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>970</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26">
-        <v>2912</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>969</v>
-      </c>
-    </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27">
-        <v>3881</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>970</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28">
-        <v>4851</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>970</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29">
-        <v>5821</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
-        <v>969</v>
-      </c>
-    </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30">
-        <v>6790</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
-        <v>970</v>
-      </c>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31">
-        <v>7760</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="0"/>
-        <v>970</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32">
-        <v>8730</v>
+      <c r="D25">
+        <f>D24/C25</f>
+        <v>1.0000152590218966E-6</v>
+      </c>
+      <c r="E25">
+        <f>D25*1000</f>
+        <v>1.0000152590218965E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1195,27 +1101,27 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="F3" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -1234,7 +1140,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -1260,27 +1166,27 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3">
         <f>D4</f>
@@ -1300,7 +1206,7 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3">
         <f>D5</f>
@@ -1320,27 +1226,27 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3">
         <f>D9</f>
@@ -1360,7 +1266,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3">
         <f>D10</f>
@@ -1399,55 +1305,55 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[main] Update files and implemented GSL/BSM Basic.
- GSL/PSM execution time is about 37us.
</commit_message>
<xml_diff>
--- a/Document/Environment.xlsx
+++ b/Document/Environment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\GSL\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723072B3-6274-485C-921C-12C6A2875443}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57D61E9-3134-4721-B9CF-F4B2DB2BC7CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1" xr2:uid="{2B8BF1E6-E496-4F89-BDC8-54DCCB78AA27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3" xr2:uid="{2B8BF1E6-E496-4F89-BDC8-54DCCB78AA27}"/>
   </bookViews>
   <sheets>
     <sheet name="Folder" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>GTK</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>1us</t>
+  </si>
+  <si>
+    <t>ISR/Thread</t>
+  </si>
+  <si>
+    <t>ICSR[0..9] M0+</t>
   </si>
 </sst>
 </file>
@@ -927,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777F88CA-E307-47AA-93AB-8788864B7E3B}">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -1292,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB75EB0-4C9A-4A63-B70A-F5FCA9A84744}">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,6 +1360,14 @@
       </c>
       <c r="C8" s="4" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[main] Update overall, implement basic feature of PSM, BSM, QUE.
</commit_message>
<xml_diff>
--- a/Document/Environment.xlsx
+++ b/Document/Environment.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\GSL\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_HKF\_dev\Repository\GSL\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57D61E9-3134-4721-B9CF-F4B2DB2BC7CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEADD7A7-A64D-49E9-90EA-5277192A8320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3" xr2:uid="{2B8BF1E6-E496-4F89-BDC8-54DCCB78AA27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2B8BF1E6-E496-4F89-BDC8-54DCCB78AA27}"/>
   </bookViews>
   <sheets>
     <sheet name="Folder" sheetId="1" r:id="rId1"/>
     <sheet name="PWM" sheetId="2" r:id="rId2"/>
     <sheet name="Resources" sheetId="4" r:id="rId3"/>
     <sheet name="Links" sheetId="3" r:id="rId4"/>
+    <sheet name="ETC" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>GTK</t>
   </si>
@@ -192,7 +193,7 @@
         <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -203,7 +204,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -222,16 +223,44 @@
   <si>
     <t>ICSR[0..9] M0+</t>
   </si>
+  <si>
+    <t>U32</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ms</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>m</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>h</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="4"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -239,7 +268,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -248,7 +277,7 @@
       <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -256,8 +285,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -320,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -348,15 +384,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -807,21 +839,21 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -829,7 +861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D4" t="s">
         <v>8</v>
       </c>
@@ -837,12 +869,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D6" t="s">
         <v>7</v>
       </c>
@@ -850,17 +882,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D9" t="s">
         <v>14</v>
       </c>
@@ -871,17 +903,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="E12" t="s">
         <v>9</v>
       </c>
@@ -889,17 +921,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
         <v>2</v>
       </c>
@@ -907,7 +939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
         <v>3</v>
       </c>
@@ -925,7 +957,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -933,29 +967,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777F88CA-E307-47AA-93AB-8788864B7E3B}">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
@@ -964,7 +998,7 @@
         <v>32000000</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
@@ -972,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>51</v>
       </c>
@@ -981,7 +1015,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
@@ -989,12 +1023,12 @@
         <v>31999</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B16" s="2" t="s">
         <v>50</v>
       </c>
@@ -1003,7 +1037,7 @@
         <v>32000000</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1011,7 +1045,7 @@
         <v>3199</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" ht="21" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
@@ -1019,21 +1053,33 @@
         <f>C16/(C19+1)/(C17+1)</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f>1/C18</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>D18/C19</f>
+        <v>1.1111111111111112E-4</v>
+      </c>
+      <c r="E19">
+        <f>D19*1000</f>
+        <v>0.11111111111111112</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
@@ -1042,7 +1088,7 @@
         <v>32000000</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
@@ -1050,7 +1096,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="21" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
@@ -1063,7 +1109,7 @@
         <v>6.5535999999999997E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
@@ -1080,6 +1126,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1094,23 +1141,23 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B2" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B3" s="11"/>
       <c r="C3" s="7" t="s">
         <v>36</v>
@@ -1125,7 +1172,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
         <v>39</v>
       </c>
@@ -1144,7 +1191,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1163,19 +1210,16 @@
         <v>0.15406249999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B7" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
         <v>36</v>
@@ -1190,7 +1234,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B9" s="5" t="s">
         <v>39</v>
       </c>
@@ -1210,7 +1254,7 @@
         <v>0.24374999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>40</v>
       </c>
@@ -1230,12 +1274,12 @@
         <v>0.21984375</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B12" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" s="12"/>
       <c r="C13" s="8" t="s">
         <v>36</v>
@@ -1250,7 +1294,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>39</v>
       </c>
@@ -1270,7 +1314,7 @@
         <v>0.24374999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B15" s="5" t="s">
         <v>40</v>
       </c>
@@ -1291,6 +1335,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1300,16 +1345,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB75EB0-4C9A-4A63-B70A-F5FCA9A84744}">
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>27</v>
       </c>
@@ -1317,7 +1362,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -1325,7 +1370,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -1333,12 +1378,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C5" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -1346,7 +1391,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>46</v>
       </c>
@@ -1354,7 +1399,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>48</v>
       </c>
@@ -1362,7 +1407,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -1371,6 +1416,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EA9B5D05-DBFA-4C86-8668-AFCCB06ECA01}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{14BA6434-DA56-48ED-A571-2C6F9634E2B9}"/>
@@ -1382,4 +1428,77 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2602AF2B-4CA4-4F72-9D8E-10355B2C37E6}">
+  <dimension ref="B2:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B3">
+        <f>POWER(2,32)</f>
+        <v>4294967296</v>
+      </c>
+      <c r="C3">
+        <f>B3/1000</f>
+        <v>4294967.2960000001</v>
+      </c>
+      <c r="D3">
+        <f>C3/1000</f>
+        <v>4294.9672959999998</v>
+      </c>
+      <c r="E3">
+        <f>D3/60</f>
+        <v>71.582788266666668</v>
+      </c>
+      <c r="F3">
+        <f>E3/60</f>
+        <v>1.1930464711111111</v>
+      </c>
+      <c r="G3">
+        <f>F3/24</f>
+        <v>4.9710269629629628E-2</v>
+      </c>
+      <c r="H3">
+        <f>G3/365</f>
+        <v>1.3619251953323185E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[main] Under consideration, GSL Pilot.
</commit_message>
<xml_diff>
--- a/Document/Environment.xlsx
+++ b/Document/Environment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_HKF\_dev\Repository\GSL\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7B7B87-1884-44AD-A381-AF2068E17229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27206E1-D209-4FBD-BAA5-8786858E9DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{2B8BF1E6-E496-4F89-BDC8-54DCCB78AA27}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="127">
   <si>
     <t>GTS</t>
   </si>
@@ -408,6 +408,106 @@
   </si>
   <si>
     <t>vidGslDiagElapsedCallback</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>PSM</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidPsmInit</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidPsmSrvc</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>BPM</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidBpmInit</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidBpmProc</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>QUEUE</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>DIAG</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidQueInit</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidDiagInit</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>enuBsmNotifyCallback</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidDiagTusAccumulate</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidBsmInit</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidBsmSrvc</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidDsmInit</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidDsmSrvc</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidLsmInit</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidLsmSrvc</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidDiagTrace</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidDiagKeepAlive</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidDiagTusStart</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>u32DiagTusElapsed</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>pstrPsmKeepAlive</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidQueEnque</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>vidQueDeque</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -486,7 +586,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +608,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -786,9 +892,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -801,7 +904,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -831,7 +934,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -864,7 +967,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -877,6 +980,66 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4349,72 +4512,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="図 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32E68E5B-5EEB-8194-7800-236C49F2FE8A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7200900" y="381000"/>
-          <a:ext cx="5972175" cy="9915525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -5245,856 +5342,1511 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{202F9C68-BA9B-415A-B4F6-E6F10680B109}">
-  <dimension ref="C3:S56"/>
+  <dimension ref="C3:AN112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE21" sqref="AE21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AO108" sqref="AO107:AO108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="5" width="3.625" style="18" customWidth="1"/>
     <col min="6" max="6" width="1.625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="24.25" style="18" customWidth="1"/>
+    <col min="7" max="7" width="26" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="3.625" style="18" customWidth="1"/>
     <col min="10" max="10" width="1.625" style="18" customWidth="1"/>
-    <col min="11" max="19" width="3.625" style="18" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="18"/>
+    <col min="11" max="13" width="3.625" style="18" customWidth="1"/>
+    <col min="14" max="14" width="1.625" style="18" customWidth="1"/>
+    <col min="15" max="15" width="10.375" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="22" width="3.625" style="18" customWidth="1"/>
+    <col min="23" max="23" width="1.625" style="18" customWidth="1"/>
+    <col min="24" max="36" width="3.625" style="18" customWidth="1"/>
+    <col min="37" max="37" width="1.625" style="18" customWidth="1"/>
+    <col min="38" max="41" width="3.625" style="18" customWidth="1"/>
+    <col min="42" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="20"/>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="L3" s="37"/>
+      <c r="L3" s="36"/>
       <c r="M3" s="20"/>
-      <c r="Q3" s="47" t="s">
+      <c r="Q3" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="R3" s="48"/>
+      <c r="R3" s="47"/>
       <c r="S3" s="20"/>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="40"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="51"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="50"/>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
       <c r="G5" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="40"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="51"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="39"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="50"/>
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
       <c r="J6" s="23"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="43"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="42"/>
       <c r="N6" s="21"/>
       <c r="O6" s="22"/>
       <c r="P6" s="23"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="51"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="50"/>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
       <c r="G7" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="40"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="51"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="39"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="50"/>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
       <c r="J8" s="23"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="43"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="42"/>
       <c r="N8" s="21"/>
       <c r="O8" s="22"/>
       <c r="P8" s="23"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="51"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="50"/>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
       <c r="G9" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="40"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="51"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="39"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="50"/>
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
       <c r="J10" s="23"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="43"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="42"/>
       <c r="N10" s="21"/>
       <c r="O10" s="22"/>
       <c r="P10" s="23"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="51"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="50"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
       <c r="G11" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="K11" s="38"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="40"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="51"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="39"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="50"/>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="43"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="42"/>
       <c r="N12" s="21"/>
       <c r="O12" s="22"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="51"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="50"/>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
       <c r="G13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="K13" s="38"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="40"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="51"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="39"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="50"/>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
       <c r="J14" s="23"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="43"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="42"/>
       <c r="N14" s="21"/>
       <c r="O14" s="22"/>
       <c r="P14" s="23"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="51"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="50"/>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
       <c r="G15" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="40"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="51"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="39"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="50"/>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="23"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="43"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="42"/>
       <c r="N16" s="21"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23"/>
-      <c r="Q16" s="52"/>
-      <c r="R16" s="53"/>
-      <c r="S16" s="54"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="52"/>
+      <c r="S16" s="53"/>
     </row>
     <row r="17" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="40"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="39"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="40"/>
-      <c r="Q18" s="47" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="39"/>
+      <c r="Q18" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="R18" s="48"/>
+      <c r="R18" s="47"/>
       <c r="S18" s="20"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
       <c r="G19" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="K19" s="38"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="40"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="50"/>
-      <c r="S19" s="51"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="39"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="50"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="21"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
       <c r="J20" s="23"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="43"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="42"/>
       <c r="N20" s="21"/>
       <c r="O20" s="22"/>
       <c r="P20" s="23"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="50"/>
-      <c r="S20" s="51"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="50"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
       <c r="G21" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K21" s="38"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="40"/>
-      <c r="Q21" s="49"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="51"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="39"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="50"/>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="21"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="23"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="43"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="42"/>
       <c r="N22" s="21"/>
       <c r="O22" s="22"/>
       <c r="P22" s="23"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="50"/>
-      <c r="S22" s="51"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="50"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
       <c r="G23" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="K23" s="38"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="40"/>
-      <c r="Q23" s="49"/>
-      <c r="R23" s="50"/>
-      <c r="S23" s="51"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="39"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="50"/>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="21"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
       <c r="J24" s="23"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="43"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="42"/>
       <c r="N24" s="21"/>
       <c r="O24" s="22"/>
       <c r="P24" s="23"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="50"/>
-      <c r="S24" s="51"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="50"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
       <c r="G25" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="K25" s="38"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="40"/>
-      <c r="Q25" s="49"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="51"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="39"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="50"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
       <c r="F26" s="21"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
       <c r="J26" s="23"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="43"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="42"/>
       <c r="N26" s="21"/>
       <c r="O26" s="22"/>
       <c r="P26" s="23"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="50"/>
-      <c r="S26" s="51"/>
+      <c r="Q26" s="48"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="50"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
       <c r="G27" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="K27" s="38"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="40"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="51"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="39"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="50"/>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="43"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="42"/>
       <c r="N28" s="21"/>
       <c r="O28" s="22"/>
       <c r="P28" s="23"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="51"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="50"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
       <c r="G29" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="K29" s="38"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="40"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="50"/>
-      <c r="S29" s="51"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="39"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="50"/>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="43"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="42"/>
       <c r="N30" s="21"/>
       <c r="O30" s="22"/>
       <c r="P30" s="23"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="50"/>
-      <c r="S30" s="51"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="50"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
       <c r="G31" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="K31" s="38"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="40"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="51"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="39"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="50"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="29"/>
       <c r="F32" s="21"/>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
       <c r="J32" s="23"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="43"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="42"/>
       <c r="N32" s="21"/>
       <c r="O32" s="22"/>
       <c r="P32" s="23"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="51"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="50"/>
     </row>
     <row r="33" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="29"/>
       <c r="G33" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="K33" s="38"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="40"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="50"/>
-      <c r="S33" s="51"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="39"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="50"/>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="21"/>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
       <c r="J34" s="23"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="43"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="42"/>
       <c r="N34" s="21"/>
       <c r="O34" s="22"/>
       <c r="P34" s="23"/>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="51"/>
+      <c r="Q34" s="48"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="50"/>
     </row>
     <row r="35" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="29"/>
       <c r="G35" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="K35" s="38"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="40"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="51"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="39"/>
+      <c r="Q35" s="48"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="50"/>
     </row>
     <row r="36" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C36" s="28"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="21"/>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
       <c r="J36" s="23"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="43"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="42"/>
       <c r="N36" s="21"/>
       <c r="O36" s="22"/>
       <c r="P36" s="23"/>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="50"/>
-      <c r="S36" s="51"/>
+      <c r="Q36" s="48"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="50"/>
     </row>
     <row r="37" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
       <c r="G37" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="K37" s="38"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="40"/>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="50"/>
-      <c r="S37" s="51"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="39"/>
+      <c r="Q37" s="48"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="50"/>
     </row>
     <row r="38" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
       <c r="J38" s="22"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="43"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="42"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
       <c r="P38" s="23"/>
-      <c r="Q38" s="52"/>
-      <c r="R38" s="53"/>
-      <c r="S38" s="54"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="52"/>
+      <c r="S38" s="53"/>
     </row>
     <row r="39" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="24"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="40"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="29"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="39"/>
     </row>
     <row r="40" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C40" s="28"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="40"/>
-      <c r="Q40" s="47" t="s">
+      <c r="C40" s="27"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="29"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="39"/>
+      <c r="Q40" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="R40" s="48"/>
+      <c r="R40" s="47"/>
       <c r="S40" s="20"/>
     </row>
     <row r="41" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C41" s="28"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="30"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29"/>
       <c r="G41" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="K41" s="38"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="40"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="50"/>
-      <c r="S41" s="51"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="39"/>
+      <c r="Q41" s="48"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="50"/>
     </row>
     <row r="42" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C42" s="28"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="30"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="29"/>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
       <c r="I42" s="22"/>
       <c r="J42" s="22"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="46"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="45"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
       <c r="P42" s="23"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="50"/>
-      <c r="S42" s="51"/>
+      <c r="Q42" s="48"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="50"/>
     </row>
     <row r="43" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="30"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="29"/>
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
     </row>
     <row r="44" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
-      <c r="K44" s="36" t="s">
+      <c r="C44" s="27"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="29"/>
+      <c r="K44" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="L44" s="37"/>
+      <c r="L44" s="36"/>
       <c r="M44" s="20"/>
-      <c r="Q44" s="24"/>
-      <c r="R44" s="24"/>
-      <c r="S44" s="24"/>
     </row>
     <row r="45" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C45" s="28"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="30"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="29"/>
       <c r="I45" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K45" s="38"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="40"/>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="24"/>
-      <c r="S45" s="24"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="39"/>
     </row>
     <row r="46" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C46" s="28"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="30"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="29"/>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
       <c r="H46" s="22"/>
       <c r="I46" s="22"/>
       <c r="J46" s="23"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="40"/>
-      <c r="Q46" s="24"/>
-      <c r="R46" s="24"/>
-      <c r="S46" s="24"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="39"/>
     </row>
     <row r="47" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C47" s="28"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="30"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="29"/>
       <c r="I47" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="K47" s="38"/>
-      <c r="L47" s="39"/>
-      <c r="M47" s="40"/>
-      <c r="Q47" s="24"/>
-      <c r="R47" s="24"/>
-      <c r="S47" s="24"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="39"/>
     </row>
     <row r="48" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C48" s="28"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="30"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="29"/>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
       <c r="H48" s="22"/>
       <c r="I48" s="22"/>
       <c r="J48" s="23"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="39"/>
-      <c r="M48" s="40"/>
-      <c r="Q48" s="24"/>
-      <c r="R48" s="24"/>
-      <c r="S48" s="24"/>
-    </row>
-    <row r="49" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C49" s="28"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="30"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="39"/>
+    </row>
+    <row r="49" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C49" s="27"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
       <c r="I49" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="K49" s="38"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="40"/>
-      <c r="Q49" s="24"/>
-      <c r="R49" s="24"/>
-      <c r="S49" s="24"/>
-    </row>
-    <row r="50" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C50" s="28"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="30"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="39"/>
+    </row>
+    <row r="50" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C50" s="27"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="29"/>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="22"/>
       <c r="I50" s="22"/>
       <c r="J50" s="23"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="39"/>
-      <c r="M50" s="40"/>
-      <c r="Q50" s="24"/>
-      <c r="R50" s="24"/>
-      <c r="S50" s="24"/>
-    </row>
-    <row r="51" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C51" s="28"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="30"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="39"/>
+    </row>
+    <row r="51" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29"/>
       <c r="I51" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="K51" s="38"/>
-      <c r="L51" s="39"/>
-      <c r="M51" s="40"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="24"/>
-    </row>
-    <row r="52" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C52" s="28"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="30"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="38"/>
+      <c r="M51" s="39"/>
+    </row>
+    <row r="52" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C52" s="27"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29"/>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
       <c r="H52" s="22"/>
       <c r="I52" s="22"/>
       <c r="J52" s="23"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="40"/>
-      <c r="Q52" s="24"/>
-      <c r="R52" s="24"/>
-      <c r="S52" s="24"/>
-    </row>
-    <row r="53" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C53" s="28"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="30"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="39"/>
+    </row>
+    <row r="53" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C53" s="27"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29"/>
       <c r="I53" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="K53" s="38"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="40"/>
-      <c r="Q53" s="24"/>
-      <c r="R53" s="24"/>
-      <c r="S53" s="24"/>
-    </row>
-    <row r="54" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="C54" s="31"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="33"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="38"/>
+      <c r="M53" s="39"/>
+    </row>
+    <row r="54" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C54" s="30"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
       <c r="H54" s="22"/>
       <c r="I54" s="22"/>
       <c r="J54" s="23"/>
-      <c r="K54" s="38"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="40"/>
-      <c r="Q54" s="24"/>
-      <c r="R54" s="24"/>
-      <c r="S54" s="24"/>
-    </row>
-    <row r="55" spans="3:19" x14ac:dyDescent="0.4">
+      <c r="K54" s="37"/>
+      <c r="L54" s="38"/>
+      <c r="M54" s="39"/>
+    </row>
+    <row r="55" spans="3:13" x14ac:dyDescent="0.4">
       <c r="K55" s="22"/>
       <c r="L55" s="22"/>
       <c r="M55" s="22"/>
-      <c r="Q55" s="24"/>
-      <c r="R55" s="24"/>
-      <c r="S55" s="24"/>
-    </row>
-    <row r="56" spans="3:19" x14ac:dyDescent="0.4">
-      <c r="Q56" s="24"/>
-      <c r="R56" s="24"/>
-      <c r="S56" s="24"/>
+    </row>
+    <row r="61" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C61" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="36"/>
+      <c r="E61" s="20"/>
+      <c r="K61" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="L61" s="47"/>
+      <c r="M61" s="20"/>
+    </row>
+    <row r="62" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C62" s="58"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="60"/>
+      <c r="G62" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="K62" s="48"/>
+      <c r="L62" s="49"/>
+      <c r="M62" s="50"/>
+    </row>
+    <row r="63" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C63" s="37"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="48"/>
+      <c r="L63" s="49"/>
+      <c r="M63" s="50"/>
+    </row>
+    <row r="64" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C64" s="37"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="39"/>
+      <c r="G64" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="K64" s="48"/>
+      <c r="L64" s="49"/>
+      <c r="M64" s="50"/>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C65" s="37"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="22"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="51"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="53"/>
+    </row>
+    <row r="66" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C66" s="37"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="39"/>
+      <c r="K66" s="22"/>
+      <c r="L66" s="22"/>
+      <c r="M66" s="22"/>
+    </row>
+    <row r="67" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C67" s="37"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="39"/>
+      <c r="K67" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="L67" s="47"/>
+      <c r="M67" s="20"/>
+    </row>
+    <row r="68" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C68" s="37"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="39"/>
+      <c r="G68" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="K68" s="48"/>
+      <c r="L68" s="49"/>
+      <c r="M68" s="50"/>
+    </row>
+    <row r="69" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C69" s="37"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="48"/>
+      <c r="L69" s="49"/>
+      <c r="M69" s="50"/>
+    </row>
+    <row r="70" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C70" s="37"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="39"/>
+      <c r="G70" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="K70" s="48"/>
+      <c r="L70" s="49"/>
+      <c r="M70" s="50"/>
+    </row>
+    <row r="71" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C71" s="37"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
+      <c r="J71" s="23"/>
+      <c r="K71" s="51"/>
+      <c r="L71" s="52"/>
+      <c r="M71" s="53"/>
+    </row>
+    <row r="72" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C72" s="37"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="39"/>
+    </row>
+    <row r="73" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C73" s="37"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="39"/>
+      <c r="K73" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="L73" s="47"/>
+      <c r="M73" s="20"/>
+    </row>
+    <row r="74" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C74" s="37"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="39"/>
+      <c r="G74" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="K74" s="48"/>
+      <c r="L74" s="49"/>
+      <c r="M74" s="50"/>
+    </row>
+    <row r="75" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C75" s="37"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="23"/>
+      <c r="K75" s="48"/>
+      <c r="L75" s="49"/>
+      <c r="M75" s="50"/>
+    </row>
+    <row r="76" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C76" s="37"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="39"/>
+      <c r="K76" s="22"/>
+      <c r="L76" s="22"/>
+      <c r="M76" s="22"/>
+    </row>
+    <row r="77" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C77" s="37"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="39"/>
+      <c r="K77" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="L77" s="47"/>
+      <c r="M77" s="20"/>
+    </row>
+    <row r="78" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C78" s="37"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="39"/>
+      <c r="G78" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="K78" s="54"/>
+      <c r="L78" s="55"/>
+      <c r="M78" s="56"/>
+    </row>
+    <row r="79" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C79" s="37"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
+      <c r="K79" s="48"/>
+      <c r="L79" s="49"/>
+      <c r="M79" s="50"/>
+    </row>
+    <row r="80" spans="3:13" x14ac:dyDescent="0.4">
+      <c r="C80" s="37"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="39"/>
+      <c r="G80" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="K80" s="48"/>
+      <c r="L80" s="49"/>
+      <c r="M80" s="50"/>
+    </row>
+    <row r="81" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C81" s="37"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="22"/>
+      <c r="J81" s="22"/>
+      <c r="K81" s="51"/>
+      <c r="L81" s="52"/>
+      <c r="M81" s="53"/>
+    </row>
+    <row r="82" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C82" s="37"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="39"/>
+    </row>
+    <row r="83" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C83" s="37"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="39"/>
+      <c r="Q83" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="R83" s="47"/>
+      <c r="S83" s="20"/>
+    </row>
+    <row r="84" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C84" s="37"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="39"/>
+      <c r="G84" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q84" s="54"/>
+      <c r="R84" s="55"/>
+      <c r="S84" s="56"/>
+    </row>
+    <row r="85" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C85" s="61"/>
+      <c r="D85" s="62"/>
+      <c r="E85" s="63"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22"/>
+      <c r="I85" s="22"/>
+      <c r="J85" s="22"/>
+      <c r="K85" s="22"/>
+      <c r="L85" s="22"/>
+      <c r="M85" s="22"/>
+      <c r="N85" s="22"/>
+      <c r="O85" s="22"/>
+      <c r="P85" s="22"/>
+      <c r="Q85" s="51"/>
+      <c r="R85" s="52"/>
+      <c r="S85" s="53"/>
+    </row>
+    <row r="89" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C89" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="D89" s="47"/>
+      <c r="E89" s="20"/>
+      <c r="K89" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="L89" s="47"/>
+      <c r="M89" s="20"/>
+      <c r="T89" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="U89" s="47"/>
+      <c r="V89" s="20"/>
+      <c r="AC89" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD89" s="47"/>
+      <c r="AE89" s="20"/>
+      <c r="AL89" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM89" s="47"/>
+      <c r="AN89" s="20"/>
+    </row>
+    <row r="90" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C90" s="64"/>
+      <c r="D90" s="65"/>
+      <c r="E90" s="66"/>
+      <c r="G90" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="K90" s="64"/>
+      <c r="L90" s="65"/>
+      <c r="M90" s="66"/>
+      <c r="O90" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="T90" s="64"/>
+      <c r="U90" s="65"/>
+      <c r="V90" s="66"/>
+      <c r="X90" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC90" s="64"/>
+      <c r="AD90" s="65"/>
+      <c r="AE90" s="66"/>
+      <c r="AJ90" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL90" s="64"/>
+      <c r="AM90" s="65"/>
+      <c r="AN90" s="66"/>
+    </row>
+    <row r="91" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C91" s="67"/>
+      <c r="D91" s="68"/>
+      <c r="E91" s="69"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="22"/>
+      <c r="J91" s="22"/>
+      <c r="K91" s="67"/>
+      <c r="L91" s="68"/>
+      <c r="M91" s="69"/>
+      <c r="N91" s="21"/>
+      <c r="O91" s="22"/>
+      <c r="P91" s="22"/>
+      <c r="Q91" s="22"/>
+      <c r="R91" s="22"/>
+      <c r="S91" s="22"/>
+      <c r="T91" s="67"/>
+      <c r="U91" s="68"/>
+      <c r="V91" s="69"/>
+      <c r="W91" s="21"/>
+      <c r="X91" s="22"/>
+      <c r="Y91" s="22"/>
+      <c r="Z91" s="22"/>
+      <c r="AA91" s="22"/>
+      <c r="AB91" s="22"/>
+      <c r="AC91" s="70"/>
+      <c r="AD91" s="71"/>
+      <c r="AE91" s="72"/>
+      <c r="AF91" s="21"/>
+      <c r="AG91" s="22"/>
+      <c r="AH91" s="22"/>
+      <c r="AI91" s="22"/>
+      <c r="AJ91" s="22"/>
+      <c r="AK91" s="22"/>
+      <c r="AL91" s="70"/>
+      <c r="AM91" s="71"/>
+      <c r="AN91" s="72"/>
+    </row>
+    <row r="92" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C92" s="67"/>
+      <c r="D92" s="68"/>
+      <c r="E92" s="69"/>
+      <c r="G92" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="K92" s="67"/>
+      <c r="L92" s="68"/>
+      <c r="M92" s="69"/>
+      <c r="N92" s="57"/>
+      <c r="O92" s="73"/>
+      <c r="P92" s="73"/>
+      <c r="Q92" s="73"/>
+      <c r="R92" s="73"/>
+      <c r="S92" s="73"/>
+      <c r="T92" s="67"/>
+      <c r="U92" s="68"/>
+      <c r="V92" s="69"/>
+    </row>
+    <row r="93" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C93" s="67"/>
+      <c r="D93" s="68"/>
+      <c r="E93" s="69"/>
+      <c r="F93" s="22"/>
+      <c r="G93" s="22"/>
+      <c r="H93" s="22"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="22"/>
+      <c r="K93" s="70"/>
+      <c r="L93" s="71"/>
+      <c r="M93" s="72"/>
+      <c r="N93" s="57"/>
+      <c r="O93" s="73"/>
+      <c r="P93" s="73"/>
+      <c r="Q93" s="73"/>
+      <c r="R93" s="73"/>
+      <c r="S93" s="73"/>
+      <c r="T93" s="67"/>
+      <c r="U93" s="68"/>
+      <c r="V93" s="69"/>
+    </row>
+    <row r="94" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C94" s="67"/>
+      <c r="D94" s="68"/>
+      <c r="E94" s="69"/>
+      <c r="T94" s="67"/>
+      <c r="U94" s="68"/>
+      <c r="V94" s="69"/>
+    </row>
+    <row r="95" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C95" s="67"/>
+      <c r="D95" s="68"/>
+      <c r="E95" s="69"/>
+      <c r="K95" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="L95" s="47"/>
+      <c r="M95" s="20"/>
+      <c r="T95" s="67"/>
+      <c r="U95" s="68"/>
+      <c r="V95" s="69"/>
+    </row>
+    <row r="96" spans="3:40" x14ac:dyDescent="0.4">
+      <c r="C96" s="67"/>
+      <c r="D96" s="68"/>
+      <c r="E96" s="69"/>
+      <c r="G96" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="K96" s="64"/>
+      <c r="L96" s="65"/>
+      <c r="M96" s="66"/>
+      <c r="O96" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="T96" s="67"/>
+      <c r="U96" s="68"/>
+      <c r="V96" s="69"/>
+    </row>
+    <row r="97" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C97" s="67"/>
+      <c r="D97" s="68"/>
+      <c r="E97" s="69"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="22"/>
+      <c r="I97" s="22"/>
+      <c r="J97" s="22"/>
+      <c r="K97" s="67"/>
+      <c r="L97" s="68"/>
+      <c r="M97" s="69"/>
+      <c r="N97" s="21"/>
+      <c r="O97" s="22"/>
+      <c r="P97" s="22"/>
+      <c r="Q97" s="22"/>
+      <c r="R97" s="22"/>
+      <c r="S97" s="22"/>
+      <c r="T97" s="67"/>
+      <c r="U97" s="68"/>
+      <c r="V97" s="69"/>
+    </row>
+    <row r="98" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C98" s="67"/>
+      <c r="D98" s="68"/>
+      <c r="E98" s="69"/>
+      <c r="G98" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="K98" s="67"/>
+      <c r="L98" s="68"/>
+      <c r="M98" s="69"/>
+      <c r="T98" s="67"/>
+      <c r="U98" s="68"/>
+      <c r="V98" s="69"/>
+    </row>
+    <row r="99" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C99" s="67"/>
+      <c r="D99" s="68"/>
+      <c r="E99" s="69"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="22"/>
+      <c r="J99" s="22"/>
+      <c r="K99" s="70"/>
+      <c r="L99" s="71"/>
+      <c r="M99" s="72"/>
+      <c r="T99" s="67"/>
+      <c r="U99" s="68"/>
+      <c r="V99" s="69"/>
+    </row>
+    <row r="100" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C100" s="67"/>
+      <c r="D100" s="68"/>
+      <c r="E100" s="69"/>
+      <c r="T100" s="67"/>
+      <c r="U100" s="68"/>
+      <c r="V100" s="69"/>
+    </row>
+    <row r="101" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C101" s="67"/>
+      <c r="D101" s="68"/>
+      <c r="E101" s="69"/>
+      <c r="K101" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="L101" s="47"/>
+      <c r="M101" s="20"/>
+      <c r="T101" s="67"/>
+      <c r="U101" s="68"/>
+      <c r="V101" s="69"/>
+    </row>
+    <row r="102" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C102" s="67"/>
+      <c r="D102" s="68"/>
+      <c r="E102" s="69"/>
+      <c r="G102" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="K102" s="64"/>
+      <c r="L102" s="65"/>
+      <c r="M102" s="66"/>
+      <c r="O102" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="T102" s="67"/>
+      <c r="U102" s="68"/>
+      <c r="V102" s="69"/>
+    </row>
+    <row r="103" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C103" s="67"/>
+      <c r="D103" s="68"/>
+      <c r="E103" s="69"/>
+      <c r="F103" s="22"/>
+      <c r="G103" s="22"/>
+      <c r="H103" s="22"/>
+      <c r="I103" s="22"/>
+      <c r="J103" s="22"/>
+      <c r="K103" s="67"/>
+      <c r="L103" s="68"/>
+      <c r="M103" s="69"/>
+      <c r="N103" s="21"/>
+      <c r="O103" s="22"/>
+      <c r="P103" s="22"/>
+      <c r="Q103" s="22"/>
+      <c r="R103" s="22"/>
+      <c r="S103" s="22"/>
+      <c r="T103" s="67"/>
+      <c r="U103" s="68"/>
+      <c r="V103" s="69"/>
+    </row>
+    <row r="104" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C104" s="67"/>
+      <c r="D104" s="68"/>
+      <c r="E104" s="69"/>
+      <c r="G104" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="K104" s="67"/>
+      <c r="L104" s="68"/>
+      <c r="M104" s="69"/>
+      <c r="T104" s="67"/>
+      <c r="U104" s="68"/>
+      <c r="V104" s="69"/>
+    </row>
+    <row r="105" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C105" s="67"/>
+      <c r="D105" s="68"/>
+      <c r="E105" s="69"/>
+      <c r="F105" s="22"/>
+      <c r="G105" s="22"/>
+      <c r="H105" s="22"/>
+      <c r="I105" s="22"/>
+      <c r="J105" s="22"/>
+      <c r="K105" s="70"/>
+      <c r="L105" s="71"/>
+      <c r="M105" s="72"/>
+      <c r="T105" s="67"/>
+      <c r="U105" s="68"/>
+      <c r="V105" s="69"/>
+    </row>
+    <row r="106" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C106" s="67"/>
+      <c r="D106" s="68"/>
+      <c r="E106" s="69"/>
+      <c r="T106" s="67"/>
+      <c r="U106" s="68"/>
+      <c r="V106" s="69"/>
+    </row>
+    <row r="107" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C107" s="67"/>
+      <c r="D107" s="68"/>
+      <c r="E107" s="69"/>
+      <c r="G107" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="T107" s="67"/>
+      <c r="U107" s="68"/>
+      <c r="V107" s="69"/>
+    </row>
+    <row r="108" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C108" s="67"/>
+      <c r="D108" s="68"/>
+      <c r="E108" s="69"/>
+      <c r="F108" s="22"/>
+      <c r="G108" s="22"/>
+      <c r="H108" s="22"/>
+      <c r="I108" s="22"/>
+      <c r="J108" s="22"/>
+      <c r="K108" s="22"/>
+      <c r="L108" s="22"/>
+      <c r="M108" s="22"/>
+      <c r="N108" s="22"/>
+      <c r="O108" s="22"/>
+      <c r="P108" s="22"/>
+      <c r="Q108" s="22"/>
+      <c r="R108" s="22"/>
+      <c r="S108" s="22"/>
+      <c r="T108" s="67"/>
+      <c r="U108" s="68"/>
+      <c r="V108" s="69"/>
+    </row>
+    <row r="109" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C109" s="67"/>
+      <c r="D109" s="68"/>
+      <c r="E109" s="69"/>
+      <c r="G109" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="T109" s="67"/>
+      <c r="U109" s="68"/>
+      <c r="V109" s="69"/>
+    </row>
+    <row r="110" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C110" s="67"/>
+      <c r="D110" s="68"/>
+      <c r="E110" s="69"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="22"/>
+      <c r="H110" s="22"/>
+      <c r="I110" s="22"/>
+      <c r="J110" s="22"/>
+      <c r="K110" s="22"/>
+      <c r="L110" s="22"/>
+      <c r="M110" s="22"/>
+      <c r="N110" s="22"/>
+      <c r="O110" s="22"/>
+      <c r="P110" s="22"/>
+      <c r="Q110" s="22"/>
+      <c r="R110" s="22"/>
+      <c r="S110" s="22"/>
+      <c r="T110" s="67"/>
+      <c r="U110" s="68"/>
+      <c r="V110" s="69"/>
+    </row>
+    <row r="111" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C111" s="67"/>
+      <c r="D111" s="68"/>
+      <c r="E111" s="69"/>
+      <c r="G111" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="T111" s="67"/>
+      <c r="U111" s="68"/>
+      <c r="V111" s="69"/>
+    </row>
+    <row r="112" spans="3:22" x14ac:dyDescent="0.4">
+      <c r="C112" s="70"/>
+      <c r="D112" s="71"/>
+      <c r="E112" s="72"/>
+      <c r="F112" s="22"/>
+      <c r="G112" s="22"/>
+      <c r="H112" s="22"/>
+      <c r="I112" s="22"/>
+      <c r="J112" s="22"/>
+      <c r="K112" s="22"/>
+      <c r="L112" s="22"/>
+      <c r="M112" s="22"/>
+      <c r="N112" s="22"/>
+      <c r="O112" s="22"/>
+      <c r="P112" s="22"/>
+      <c r="Q112" s="22"/>
+      <c r="R112" s="22"/>
+      <c r="S112" s="22"/>
+      <c r="T112" s="70"/>
+      <c r="U112" s="71"/>
+      <c r="V112" s="72"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>